<commit_message>
trained modelgit add .!
</commit_message>
<xml_diff>
--- a/experiments/NTU-RGB-D-CV/HCN01/best_accuracy_series.xlsx
+++ b/experiments/NTU-RGB-D-CV/HCN01/best_accuracy_series.xlsx
@@ -413,13 +413,83 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>epoch50</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>epoch100</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>epoch150</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>epoch200</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>epoch250</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>epoch300</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>epoch350</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>epoch400</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="n">
+        <v>16.79890526307596</v>
+      </c>
+      <c r="C2" t="n">
+        <v>13.649135908565</v>
+      </c>
+      <c r="D2" t="n">
+        <v>12.14348361701578</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11.22498699539417</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10.99800219809687</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10.80918658424068</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10.70239408998876</v>
+      </c>
+      <c r="I2" t="n">
+        <v>10.6191528004569</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>